<commit_message>
Update BrickPicker.py, layout.xlsx, and ~$layout.xlsx
</commit_message>
<xml_diff>
--- a/Brickpicker/layout.xlsx
+++ b/Brickpicker/layout.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t>Bild</t>
   </si>
@@ -48,15 +48,9 @@
     <t>Selection</t>
   </si>
   <si>
-    <t>ID</t>
-  </si>
-  <si>
     <t>Color</t>
   </si>
   <si>
-    <t>Unknown (0, 51, 178)</t>
-  </si>
-  <si>
     <t>Green (0, 255, 0)</t>
   </si>
   <si>
@@ -72,26 +66,17 @@
     <t>#whole color, all bricks which exist in this color</t>
   </si>
   <si>
-    <t>Whole Color</t>
-  </si>
-  <si>
-    <t>Whole Category</t>
-  </si>
-  <si>
-    <t>#whole category</t>
-  </si>
-  <si>
-    <t>Green Bricks</t>
-  </si>
-  <si>
     <t>#all green parts in cat. 3</t>
+  </si>
+  <si>
+    <t>Brick ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,6 +109,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -176,16 +167,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -492,27 +484,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G30"/>
+  <dimension ref="B2:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="3" max="3" width="14.4609375" customWidth="1"/>
+    <col min="4" max="4" width="7.07421875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.4609375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="6"/>
     </row>
     <row r="3" spans="2:3" ht="59.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
@@ -542,18 +535,18 @@
       <c r="B8" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="10" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -562,10 +555,10 @@
         <v>3</v>
       </c>
       <c r="D21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" t="s">
         <v>10</v>
-      </c>
-      <c r="E21" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.4">
@@ -578,83 +571,57 @@
       <c r="D22">
         <v>1234</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G22" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B23" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C23" t="s">
         <v>7</v>
       </c>
-      <c r="D23">
-        <v>3</v>
-      </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="7" t="s">
         <v>12</v>
       </c>
       <c r="G23" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B24" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24">
-        <v>4</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="G24" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B25" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C25" t="s">
         <v>7</v>
       </c>
-      <c r="D25">
-        <v>3</v>
-      </c>
       <c r="E25" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G25" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B26" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26">
-        <v>3</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="E30" s="5"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="E29" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>